<commit_message>
Stok guncelleme rotasi eklendi ve ilk rota bozulmadi
</commit_message>
<xml_diff>
--- a/stok/stok_guncelleme.xlsx
+++ b/stok/stok_guncelleme.xlsx
@@ -1105,7 +1105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Barkod</t>
   </si>
@@ -1125,7 +1125,13 @@
 3) Bir barkod için ürün adı değişikliğini bu şablon üzerinden yapamazsınız. Ürün adı değişikliği için Ürün Listesi sayfasına giderek ve Detaylar butonuna tıklayarak güncelleme işlemini gerçekleştirebilirseniz</t>
   </si>
   <si>
+    <t>="ZDX"&amp;T2&amp;0&amp;U2</t>
+  </si>
+  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>="ZDX"&amp;T417&amp;0&amp;U417</t>
   </si>
   <si>
     <t xml:space="preserve">Kadın </t>
@@ -1947,7 +1953,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <scheme val="minor"/>
+        <scheme val="none"/>
         <charset val="134"/>
         <family val="0"/>
         <b val="0"/>
@@ -1976,7 +1982,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Güncelleme Bilgileri-style" pivot="0" count="2" xr9:uid="{E9D803E3-8413-4E6E-9846-0D335704AC6A}">
+    <tableStyle name="Güncelleme Bilgileri-style" pivot="0" count="2" xr9:uid="{C7094BB6-8AF6-4113-B32F-AC64880C0659}">
       <tableStyleElement type="firstRowStripe" dxfId="2"/>
       <tableStyleElement type="secondRowStripe" dxfId="1"/>
     </tableStyle>
@@ -2211,8 +2217,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A417" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -2260,9 +2266,8 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" ht="18" spans="1:21">
-      <c r="A2" s="8" t="str">
-        <f t="shared" ref="A2:A440" si="0">"ZDX"&amp;T2&amp;0&amp;U2</f>
-        <v>ZDX-0148</v>
+      <c r="A2" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2283,7 +2288,7 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U2" s="14">
         <v>148</v>
@@ -2291,7 +2296,7 @@
     </row>
     <row r="3" ht="18" spans="1:21">
       <c r="A3" s="8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A2:A440" si="0">"ZDX"&amp;T3&amp;0&amp;U3</f>
         <v>ZDX0149</v>
       </c>
       <c r="B3" s="9"/>
@@ -7511,9 +7516,8 @@
       </c>
     </row>
     <row r="417" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A417" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v>ZDX0</v>
+      <c r="A417" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="B417" s="9"/>
       <c r="C417" s="9"/>
@@ -12294,10 +12298,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1">
         <v>0</v>
@@ -12305,10 +12309,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -12316,10 +12320,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>8</v>
@@ -12327,10 +12331,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>18</v>
@@ -12338,12 +12342,12 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Son Duzeltme: Sadece A sutununa dokunuldu (B ve C kaldirildi).
</commit_message>
<xml_diff>
--- a/stok/stok_guncelleme.xlsx
+++ b/stok/stok_guncelleme.xlsx
@@ -1105,7 +1105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Barkod</t>
   </si>
@@ -1125,13 +1125,7 @@
 3) Bir barkod için ürün adı değişikliğini bu şablon üzerinden yapamazsınız. Ürün adı değişikliği için Ürün Listesi sayfasına giderek ve Detaylar butonuna tıklayarak güncelleme işlemini gerçekleştirebilirseniz</t>
   </si>
   <si>
-    <t>="ZDX"&amp;T2&amp;0&amp;U2</t>
-  </si>
-  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>="ZDX"&amp;T417&amp;0&amp;U417</t>
   </si>
   <si>
     <t xml:space="preserve">Kadın </t>
@@ -1953,7 +1947,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
-        <scheme val="none"/>
+        <scheme val="minor"/>
         <charset val="134"/>
         <family val="0"/>
         <b val="0"/>
@@ -1982,7 +1976,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Güncelleme Bilgileri-style" pivot="0" count="2" xr9:uid="{C7094BB6-8AF6-4113-B32F-AC64880C0659}">
+    <tableStyle name="Güncelleme Bilgileri-style" pivot="0" count="2" xr9:uid="{2BCCBADF-FB22-4F1B-BBC3-40799CA22B73}">
       <tableStyleElement type="firstRowStripe" dxfId="2"/>
       <tableStyleElement type="secondRowStripe" dxfId="1"/>
     </tableStyle>
@@ -2218,7 +2212,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4285714285714" defaultRowHeight="15" customHeight="1"/>
@@ -2266,8 +2260,9 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" ht="18" spans="1:21">
-      <c r="A2" s="8" t="s">
-        <v>5</v>
+      <c r="A2" s="8" t="str">
+        <f t="shared" ref="A2:A440" si="0">"ZDX"&amp;T2&amp;0&amp;U2</f>
+        <v>ZDX-0148</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2288,7 +2283,7 @@
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
       <c r="T2" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U2" s="14">
         <v>148</v>
@@ -2296,7 +2291,7 @@
     </row>
     <row r="3" ht="18" spans="1:21">
       <c r="A3" s="8" t="str">
-        <f t="shared" ref="A2:A440" si="0">"ZDX"&amp;T3&amp;0&amp;U3</f>
+        <f t="shared" si="0"/>
         <v>ZDX0149</v>
       </c>
       <c r="B3" s="9"/>
@@ -7516,8 +7511,9 @@
       </c>
     </row>
     <row r="417" ht="15.75" customHeight="1" spans="1:4">
-      <c r="A417" s="8" t="s">
-        <v>7</v>
+      <c r="A417" s="8" t="str">
+        <f t="shared" si="0"/>
+        <v>ZDX0</v>
       </c>
       <c r="B417" s="9"/>
       <c r="C417" s="9"/>
@@ -12298,10 +12294,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1">
         <v>0</v>
@@ -12309,10 +12305,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -12320,10 +12316,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>8</v>
@@ -12331,10 +12327,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <v>18</v>
@@ -12342,12 +12338,12 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>